<commit_message>
Added QOL features and serialisation features
</commit_message>
<xml_diff>
--- a/FrameExtractor/TestPath.xlsx
+++ b/FrameExtractor/TestPath.xlsx
@@ -71,13 +71,37 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E1: (M) Children wearing Tall Kid with white pants at 00:00:00, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">E1: (M) Re-entry Customer wearing Black Jeans White Pants at 11:12:12, </t>
+    <t>AU045</t>
+  </si>
+  <si>
+    <t>KR045</t>
+  </si>
+  <si>
+    <t>KR054</t>
+  </si>
+  <si>
+    <t>KR055-01</t>
+  </si>
+  <si>
+    <t>KR055-02</t>
+  </si>
+  <si>
+    <t>KR057</t>
+  </si>
+  <si>
+    <t>KR062</t>
+  </si>
+  <si>
+    <t>MO002-02</t>
+  </si>
+  <si>
+    <t>SG070</t>
+  </si>
+  <si>
+    <t>TH070</t>
+  </si>
+  <si>
+    <t>VN002</t>
   </si>
 </sst>
 </file>
@@ -477,69 +501,120 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="K3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>14</v>
+      </c>
+      <c r="B4">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
+      <c r="K8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="K9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>21</v>
+      </c>
+      <c r="K12" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>